<commit_message>
Bài 29 - DataProvider TestNG
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/LoginCRM.xlsx
+++ b/src/test/resources/testdata/LoginCRM.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANHTESTER\SeleniumJava\Viettel_VTCC_SeleniumJava\VTCC_SeleniumTestNGParallel\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B53F6E-E840-40F6-B791-B820E2E42F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3998A32-EB73-4229-BE43-048358FD69D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6852" yWindow="1944" windowWidth="22704" windowHeight="13872" xr2:uid="{63FB0895-17B9-4C29-A939-325558B2FE0A}"/>
+    <workbookView xWindow="7200" yWindow="2292" windowWidth="22704" windowHeight="13872" activeTab="1" xr2:uid="{63FB0895-17B9-4C29-A939-325558B2FE0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="LoginSuccess" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="13">
   <si>
     <t>EMAIL</t>
   </si>
@@ -73,13 +73,15 @@
   </si>
   <si>
     <t>Passed</t>
+  </si>
+  <si>
+    <t>123456</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="14"/>
@@ -99,7 +101,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -119,15 +121,7 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill/>
-    </fill>
-    <fill>
-      <patternFill>
-        <bgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill>
+      <patternFill patternType="none">
         <fgColor indexed="9"/>
         <bgColor indexed="11"/>
       </patternFill>
@@ -146,43 +140,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -520,15 +488,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00F52522-4353-4632-A41B-92C95F5A080D}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.0"/>
-    <col min="2" max="2" customWidth="true" width="22.3046875"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.23046875"/>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="22.3046875" customWidth="1"/>
+    <col min="3" max="3" width="11.23046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -546,61 +514,61 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="0">
+      <c r="C2">
         <v>123456</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="0">
+      <c r="C3">
         <v>123456</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="0">
+      <c r="C4">
         <v>123456</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="0">
+      <c r="C5">
         <v>123</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -622,17 +590,92 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1CB299E-AB71-48BB-801F-5CB186865A94}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="15.69140625"/>
+    <col min="1" max="1" width="24.3828125" customWidth="1"/>
+    <col min="2" max="2" width="15.69140625" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{54508D0F-133A-47FD-B752-99B199D79960}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{DCAEC362-52DB-487E-9137-CED7E1AC7DEE}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{249043BB-C82D-44B3-BB49-57F2D84DA1DC}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{499AEACD-DAEE-482F-98C3-4A4EDD54B8C2}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{9DDDC960-753B-48C8-B195-9FF7A5FA47F1}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{57741939-343F-4FE5-BF10-74ADF4924271}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{67CC878E-F694-416C-A846-869AD2351071}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Bai 31 32 Test Listener and Log4j
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/LoginCRM.xlsx
+++ b/src/test/resources/testdata/LoginCRM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANHTESTER\SeleniumJava\Viettel_VTCC_SeleniumJava\VTCC_SeleniumTestNGParallel\src\test\resources\testdata\"/>
     </mc:Choice>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="13">
   <si>
     <t>EMAIL</t>
   </si>
@@ -82,6 +82,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="14"/>
@@ -101,7 +102,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,6 +127,20 @@
         <bgColor indexed="11"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill/>
+    </fill>
+    <fill>
+      <patternFill>
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="9"/>
+        <bgColor indexed="11"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -140,7 +155,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -151,6 +166,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -494,9 +524,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="22.3046875" customWidth="1"/>
-    <col min="3" max="3" width="11.23046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="30.0"/>
+    <col min="2" max="2" customWidth="true" width="22.3046875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.23046875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -514,27 +544,27 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="0">
         <v>123456</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="0">
         <v>123456</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -542,11 +572,11 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>7</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4">
+      <c r="C4" s="0">
         <v>123456</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -554,27 +584,29 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="0">
         <v>123</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="8" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -598,8 +630,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.3828125" customWidth="1"/>
-    <col min="2" max="2" width="15.69140625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="24.3828125"/>
+    <col min="2" max="2" customWidth="true" width="15.69140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Bài 33 34 - Extent Report - Allure Report
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/LoginCRM.xlsx
+++ b/src/test/resources/testdata/LoginCRM.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="13">
   <si>
     <t>EMAIL</t>
   </si>
@@ -155,7 +155,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -166,6 +166,78 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -553,7 +625,7 @@
       <c r="C2" s="0">
         <v>123456</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="32" t="s">
         <v>11</v>
       </c>
     </row>
@@ -593,7 +665,7 @@
       <c r="C5" s="0">
         <v>123</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="33" t="s">
         <v>11</v>
       </c>
     </row>
@@ -604,7 +676,7 @@
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="34" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>